<commit_message>
release candidate for 1.8 series
https://github.com/linkml/linkml-model/releases/tag/v1.8.0rc1
</commit_message>
<xml_diff>
--- a/linkml_runtime/linkml_model/excel/meta.xlsx
+++ b/linkml_runtime/linkml_model/excel/meta.xlsx
@@ -15,30 +15,32 @@
     <sheet name="enum_expression" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="anonymous_enum_expression" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="enum_definition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="match_query" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="reachability_query" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="structured_alias" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="path_expression" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="anonymous_slot_expression" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="slot_definition" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="anonymous_class_expression" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="class_definition" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="class_rule" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="array_expression" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="dimension_expression" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="pattern_expression" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="import_expression" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="setting" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="prefix" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="local_name" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="example" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="alt_description" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="permissible_value" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="unique_key" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="UnitOfMeasure" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="annotation" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="AnyValue" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="extension" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="enum_binding" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="match_query" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="reachability_query" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="structured_alias" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="path_expression" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="anonymous_slot_expression" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="slot_definition" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="anonymous_class_expression" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="class_definition" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="class_rule" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="array_expression" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="dimension_expression" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="pattern_expression" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="import_expression" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="setting" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="prefix" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="local_name" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="example" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="alt_description" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="permissible_value" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="unique_key" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="type_mapping" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="UnitOfMeasure" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="annotation" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="AnyValue" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="extension" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,7 +464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,32 +475,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>identifier_pattern</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>source_ontology</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>source_nodes</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>relationship_types</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>is_direct</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>include_self</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>traverse_up</t>
         </is>
       </c>
     </row>
@@ -513,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +506,57 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_ontology</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source_nodes</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>relationship_types</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>is_direct</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>include_self</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>traverse_up</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>literal_form</t>
         </is>
       </c>
@@ -539,170 +572,175 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>alias_contexts</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -718,7 +756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -954,13 +992,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ1"/>
+  <dimension ref="A1:BL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,295 +1024,305 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>required</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>recommended</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>multivalued</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>inlined</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>inlined_as_list</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>minimum_value</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>maximum_value</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>pattern</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>structured_pattern</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>implicit_prefix</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>value_presence</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>equals_string</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>equals_string_in</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>equals_number</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>equals_expression</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>exact_cardinality</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>minimum_cardinality</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>maximum_cardinality</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>has_member</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>all_members</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1282,7 +1330,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1290,13 +1338,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DK1"/>
+  <dimension ref="A1:DM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1322,560 +1370,570 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>inherited</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>readonly</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ifabsent</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>list_elements_unique</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>list_elements_ordered</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>shared</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>key</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>designates_type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>domain_of</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>subproperty_of</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>symmetric</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>reflexive</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>locally_reflexive</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>irreflexive</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>asymmetric</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>transitive</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>is_class_field</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>transitive_form_of</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>reflexive_transitive_form_of</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>is_usage_slot</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>usage_slot_name</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>relational_role</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>slot_group</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>is_grouping_slot</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>path_rule</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>disjoint_with</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>children_are_mutually_disjoint</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>union_of</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>type_mappings</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>range</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>enum_range</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>recommended</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
           <t>multivalued</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>array</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inherited</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>readonly</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ifabsent</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>list_elements_unique</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>list_elements_ordered</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>shared</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>key</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>designates_type</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>alias</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>domain_of</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>subproperty_of</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>symmetric</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>reflexive</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>locally_reflexive</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>irreflexive</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>asymmetric</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>transitive</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>inverse</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>is_class_field</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>reflexive_transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>role</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>is_usage_slot</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>usage_slot_name</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>relational_role</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>slot_group</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>is_grouping_slot</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>path_rule</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>disjoint_with</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>children_are_mutually_disjoint</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>union_of</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>range</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>range_expression</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>enum_range</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>required</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>recommended</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>inlined</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>inlined_as_list</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>minimum_value</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>maximum_value</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>pattern</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>structured_pattern</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>implicit_prefix</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>value_presence</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>equals_string</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>equals_string_in</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>equals_number</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>equals_expression</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>exact_cardinality</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>minimum_cardinality</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>maximum_cardinality</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>has_member</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>all_members</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="BS1" t="inlineStr">
+      <c r="BU1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="BT1" t="inlineStr">
+      <c r="BV1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="BU1" t="inlineStr">
+      <c r="BW1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="BV1" t="inlineStr">
+      <c r="BX1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="BW1" t="inlineStr">
+      <c r="BY1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="BX1" t="inlineStr">
+      <c r="BZ1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="BY1" t="inlineStr">
+      <c r="CA1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="BZ1" t="inlineStr">
+      <c r="CB1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="CA1" t="inlineStr">
+      <c r="CC1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="CB1" t="inlineStr">
+      <c r="CD1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="CC1" t="inlineStr">
+      <c r="CE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="CD1" t="inlineStr">
+      <c r="CF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="CE1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="CF1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="CG1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="CV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="CW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="CX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="CY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="DI1" t="inlineStr">
+      <c r="DK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="DJ1" t="inlineStr">
+      <c r="DL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="DK1" t="inlineStr">
+      <c r="DM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1883,10 +1941,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="AF2:AF1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AE2:AE1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SUBJECT,OBJECT,PREDICATE,NODE,OTHER_ROLE"</formula1>
     </dataValidation>
-    <dataValidation sqref="AZ2:AZ1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="BB2:BB1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1894,7 +1952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2120,7 +2178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2491,7 +2549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2707,227 +2765,6 @@
         </is>
       </c>
       <c r="AO1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AN1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>exact_number_dimensions</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimum_number_dimensions</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximum_number_dimensions</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_extra_dimensions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>dimensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2955,22 +2792,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>alias</t>
+          <t>exact_number_dimensions</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>maximum_cardinality</t>
+          <t>minimum_number_dimensions</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>minimum_cardinality</t>
+          <t>maximum_number_dimensions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>exact_cardinality</t>
+          <t>dimensions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -3160,7 +2997,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BL1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3276,215 +3113,220 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -3501,7 +3343,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3512,190 +3354,195 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>syntax</t>
+          <t>alias</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>interpolated</t>
+          <t>maximum_cardinality</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>partial_match</t>
+          <t>minimum_cardinality</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -3723,17 +3570,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>import_from</t>
+          <t>syntax</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>import_as</t>
+          <t>interpolated</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>import_map</t>
+          <t>partial_match</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -3923,7 +3770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3934,12 +3781,192 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>setting_key</t>
+          <t>import_from</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>setting_value</t>
+          <t>import_as</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>import_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
@@ -3965,12 +3992,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>prefix_prefix</t>
+          <t>setting_key</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>prefix_reference</t>
+          <t>setting_value</t>
         </is>
       </c>
     </row>
@@ -3996,12 +4023,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>local_name_source</t>
+          <t>prefix_prefix</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>local_name_value</t>
+          <t>prefix_reference</t>
         </is>
       </c>
     </row>
@@ -4011,6 +4038,37 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>local_name_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>local_name_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4046,7 +4104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4077,7 +4135,238 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AP1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>meaning</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>instantiates</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>implements</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mixins</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4094,34 +4383,34 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>unique_key_name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>unique_key_slots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>consider_nulls_inequal</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>meaning</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
       <c r="G1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
@@ -4280,278 +4569,6 @@
       <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AL1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>unique_key_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>unique_key_slots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>consider_nulls_inequal</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>symbol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>abbreviation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>descriptive_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ucum_code</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>derivation</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantity_kind</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>iec61360code</t>
         </is>
       </c>
     </row>
@@ -4652,6 +4669,278 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>framework_key</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapped_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>string_serialization</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>abbreviation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descriptive_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ucum_code</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>derivation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_quantity_kind</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>iec61360code</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4687,7 +4976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4705,7 +4994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5807,7 +6096,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5818,16 +6107,209 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>identifier_pattern</t>
+          <t>range</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>source_ontology</t>
+          <t>obligation_level</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>binds_value_of</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pv_formula</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"REQUIRED,RECOMMENDED,OPTIONAL,EXAMPLE,DISCOURAGED"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
linkml-model-1.9.x series release candidate
</commit_message>
<xml_diff>
--- a/linkml_runtime/linkml_model/excel/meta.xlsx
+++ b/linkml_runtime/linkml_model/excel/meta.xlsx
@@ -7,40 +7,41 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Anything" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="schema_definition" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="anonymous_type_expression" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="type_definition" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="subset_definition" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="enum_expression" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="anonymous_enum_expression" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="enum_definition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="enum_binding" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="match_query" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="reachability_query" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="structured_alias" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="path_expression" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="anonymous_slot_expression" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="slot_definition" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="anonymous_class_expression" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="class_definition" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="class_rule" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="array_expression" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="dimension_expression" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="pattern_expression" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="import_expression" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="setting" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="prefix" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="local_name" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="example" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="alt_description" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="permissible_value" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="unique_key" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="type_mapping" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="UnitOfMeasure" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="annotation" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="AnyValue" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="extension" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="AnyValue" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="extension" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="annotation" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="UnitOfMeasure" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Anything" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="schema_definition" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="anonymous_type_expression" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="type_definition" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="subset_definition" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="enum_expression" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="anonymous_enum_expression" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="enum_definition" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="enum_binding" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="match_query" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="reachability_query" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="structured_alias" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="path_expression" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="anonymous_slot_expression" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="slot_definition" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="anonymous_class_expression" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="class_definition" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="class_rule" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="array_expression" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="dimension_expression" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="pattern_expression" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="import_expression" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="setting" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="prefix" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="local_name" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="example" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="alt_description" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="permissible_value" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="unique_key" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="type_mapping" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="extra_slots_expression" sheetId="35" state="visible" r:id="rId35"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -464,6 +465,728 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>code_set</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code_set_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>code_set_version</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pv_formula</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>permissible_values</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>minus</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>inherits</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>reachable_from</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>matches</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>concepts</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>code_set</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code_set_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>code_set_version</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pv_formula</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>permissible_values</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>minus</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>inherits</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>reachable_from</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>matches</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>concepts</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BJ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>enum_uri</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code_set</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>code_set_tag</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>code_set_version</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>pv_formula</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>permissible_values</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>minus</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>inherits</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>reachable_from</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>matches</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>concepts</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>abstract</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>mixin</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>mixins</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>apply_to</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>values_from</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>string_serialization</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>id_prefixes</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>id_prefixes_are_closed</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>definition_uri</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>local_names</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>conforms_to</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>implements</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>instantiates</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>range</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>obligation_level</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>binds_value_of</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pv_formula</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"REQUIRED,RECOMMENDED,OPTIONAL,EXAMPLE,DISCOURAGED"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -489,7 +1212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -540,7 +1263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -756,7 +1479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -992,13 +1715,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BL1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1154,175 +1877,180 @@
       </c>
       <c r="AD1" t="inlineStr">
         <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1338,7 +2066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1370,322 +2098,322 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>inherited</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>readonly</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ifabsent</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>list_elements_unique</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>list_elements_ordered</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>shared</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>key</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>designates_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>domain_of</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>subproperty_of</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>symmetric</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>reflexive</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>locally_reflexive</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>irreflexive</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>asymmetric</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>transitive</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>is_class_field</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>transitive_form_of</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>reflexive_transitive_form_of</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>is_usage_slot</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>usage_slot_name</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>relational_role</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>slot_group</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>is_grouping_slot</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>path_rule</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>disjoint_with</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>children_are_mutually_disjoint</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>union_of</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>type_mappings</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>range</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>enum_range</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>recommended</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>multivalued</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>inlined</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>inlined_as_list</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>minimum_value</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>maximum_value</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>pattern</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>structured_pattern</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>implicit_prefix</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>value_presence</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>equals_string</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>equals_string_in</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>equals_number</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>equals_expression</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>minimum_cardinality</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>maximum_cardinality</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>has_member</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>all_members</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>none_of</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>exactly_one_of</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>any_of</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>all_of</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
+        <is>
           <t>array</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>inherited</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>readonly</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>ifabsent</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>list_elements_unique</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>list_elements_ordered</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>shared</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>key</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>designates_type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>alias</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>domain_of</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>subproperty_of</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>symmetric</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>reflexive</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>locally_reflexive</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>irreflexive</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>asymmetric</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>transitive</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>inverse</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>is_class_field</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>reflexive_transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>role</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>is_usage_slot</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>usage_slot_name</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>relational_role</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>slot_group</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>is_grouping_slot</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>path_rule</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>disjoint_with</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>children_are_mutually_disjoint</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>union_of</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>type_mappings</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>range</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>range_expression</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>enum_range</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bindings</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>required</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>recommended</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>multivalued</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>inlined</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>inlined_as_list</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>minimum_value</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>maximum_value</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>pattern</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>structured_pattern</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>implicit_prefix</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>value_presence</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>equals_string</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>equals_string_in</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>equals_number</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>equals_expression</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>exact_cardinality</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>minimum_cardinality</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>maximum_cardinality</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>has_member</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>all_members</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>none_of</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>exactly_one_of</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>any_of</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>all_of</t>
         </is>
       </c>
       <c r="BP1" t="inlineStr">
@@ -1941,10 +2669,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="AE2:AE1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AD2:AD1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SUBJECT,OBJECT,PREDICATE,NODE,OTHER_ROLE"</formula1>
     </dataValidation>
-    <dataValidation sqref="BB2:BB1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="BA2:BA1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1952,7 +2680,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>extension_tag</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>extension_value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2178,13 +2942,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BR1"/>
+  <dimension ref="A1:BT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2270,275 +3034,285 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>extra_slots</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>slot_conditions</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2549,7 +3323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2775,7 +3549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2991,353 +3765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BM1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>imports</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>prefixes</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>emit_prefixes</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>default_curi_maps</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>default_prefix</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>default_range</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>subsets</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>types</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>enums</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>slot_definitions</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>classes</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>metamodel_version</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>source_file</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>source_file_date</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>source_file_size</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>generation_date</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>slot_names_unique</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>settings</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>bindings</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>id_prefixes</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>id_prefixes_are_closed</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>definition_uri</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>local_names</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>conforms_to</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>implements</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>instantiates</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3553,7 +3981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3764,7 +4192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3967,135 +4395,6 @@
       <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>setting_key</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>setting_value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>prefix_prefix</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>prefix_reference</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>local_name_source</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>local_name_value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value_description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value_object</t>
         </is>
       </c>
     </row>
@@ -4121,12 +4420,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>alt_description_source</t>
+          <t>setting_key</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>alt_description_text</t>
+          <t>setting_value</t>
         </is>
       </c>
     </row>
@@ -4136,6 +4435,176 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>prefix_prefix</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>prefix_reference</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>local_name_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>local_name_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>extension_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>extension_value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value_description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value_object</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alt_description_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alt_description_text</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4366,7 +4835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4577,93 +5046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>pattern</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>structured_pattern</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>implicit_prefix</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>equals_string</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>equals_string_in</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>equals_number</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>minimum_value</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>maximum_value</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>none_of</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>exactly_one_of</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>any_of</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>all_of</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4874,7 +5257,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>allowed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4935,48 +5349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>extension_tag</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>extension_value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4994,13 +5367,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5011,17 +5384,327 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>extension_tag</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>extension_value</t>
+          <t>version</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>prefixes</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>emit_prefixes</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>default_curi_maps</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>default_prefix</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>default_range</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>subsets</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>types</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>enums</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>slot_definitions</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>classes</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>metamodel_version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>source_file</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source_file_date</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>source_file_size</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>generation_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>slot_names_unique</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>id_prefixes</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>id_prefixes_are_closed</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>definition_uri</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>local_names</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>conforms_to</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>implements</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>instantiates</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
           <t>extensions</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
@@ -5030,7 +5713,93 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>pattern</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>structured_pattern</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>implicit_prefix</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>equals_string</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>equals_string_in</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>equals_number</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>minimum_value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>maximum_value</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>none_of</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>exactly_one_of</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>any_of</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>all_of</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5356,7 +6125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5590,726 +6359,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>code_set</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>code_set_tag</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>code_set_version</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>pv_formula</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>permissible_values</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>include</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>minus</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>inherits</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>reachable_from</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>matches</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>concepts</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>code_set</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>code_set_tag</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>code_set_version</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>pv_formula</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>permissible_values</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>include</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>minus</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>inherits</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>reachable_from</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>matches</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>concepts</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BJ1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>enum_uri</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>code_set</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>code_set_tag</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>code_set_version</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>pv_formula</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>permissible_values</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>include</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>minus</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>inherits</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>reachable_from</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>matches</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>concepts</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>is_a</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>abstract</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>mixin</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>mixins</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>apply_to</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>values_from</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>string_serialization</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>id_prefixes</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>id_prefixes_are_closed</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>definition_uri</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>local_names</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>conforms_to</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>implements</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>instantiates</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AM1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>range</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>obligation_level</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>binds_value_of</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>pv_formula</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"REQUIRED,RECOMMENDED,OPTIONAL,EXAMPLE,DISCOURAGED"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>